<commit_message>
criacao do delete por id e listar todos
</commit_message>
<xml_diff>
--- a/technical_report.xlsx
+++ b/technical_report.xlsx
@@ -26,16 +26,16 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Fulano</t>
+    <t>Angelina</t>
   </si>
   <si>
-    <t>Smartphone</t>
+    <t>Celular Android</t>
   </si>
   <si>
-    <t>deu pau</t>
+    <t>não liga</t>
   </si>
   <si>
-    <t>compra outro</t>
+    <t>caiu na agua</t>
   </si>
 </sst>
 </file>
@@ -43,13 +43,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <b val="true"/>
     </font>
   </fonts>
   <fills count="2">
@@ -72,8 +77,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -86,23 +92,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="7.17578125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="12.32421875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="8.52734375" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="13.4609375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="8.8125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="14.9609375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="8.953125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="14.65625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="1">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="1">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="1">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="1">
         <v>3</v>
       </c>
     </row>

</xml_diff>